<commit_message>
update all models to latest
</commit_message>
<xml_diff>
--- a/keast-bladder/source/keast-bladder.xlsx
+++ b/keast-bladder/source/keast-bladder.xlsx
@@ -14356,7 +14356,7 @@
       </c>
       <c r="D108" s="18"/>
       <c r="E108" s="162" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="F108" s="18" t="s">
         <v>1092</v>
@@ -14387,7 +14387,7 @@
       </c>
       <c r="D109" s="18"/>
       <c r="E109" s="162" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="F109" s="18" t="s">
         <v>1092</v>
@@ -16199,7 +16199,7 @@
       <c r="B4" s="3" t="s">
         <v>1305</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>1306</v>
       </c>
       <c r="D4" s="171" t="s">

</xml_diff>